<commit_message>
correcting date problem in 3a/3b
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_hbrown_07.17.19.xlsx
+++ b/bioSample/bioSample_hbrown_07.17.19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9705A86-C5FB-E846-A83D-D8B67BF4F81B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28080790-D5C1-C248-8FDD-A86AE027BFDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22860" windowHeight="13440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>